<commit_message>
Fixed selection, updated templates
</commit_message>
<xml_diff>
--- a/templates/Epi_P6_vs_WT_Pairwise_Exact_Test_deg_template.xlsx
+++ b/templates/Epi_P6_vs_WT_Pairwise_Exact_Test_deg_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Documents/23Feb2022_Pax6_Study_DEG_Analysis/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0BB550-EE5B-EC4B-AEAA-9580CA65BD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2DEBC0-5AFD-4448-A209-14FE971AB857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="5820" windowWidth="35840" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="500" windowWidth="35840" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Description" sheetId="1" r:id="rId1"/>
@@ -414,11 +414,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -426,9 +429,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F93"/>
+  <dimension ref="B1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -770,55 +770,55 @@
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="2:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
@@ -844,56 +844,56 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="2:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="2:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
@@ -902,53 +902,53 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="14" t="s">
         <v>57</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="4" t="s">
         <v>59</v>
       </c>
@@ -961,11 +961,11 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
@@ -1022,23 +1022,23 @@
       <c r="B29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="16"/>
       <c r="E30" s="10" t="s">
         <v>22</v>
       </c>
@@ -1048,144 +1048,144 @@
       <c r="B31" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17" t="s">
+      <c r="D34" s="17"/>
+      <c r="E34" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="17"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17" t="s">
+      <c r="D35" s="17"/>
+      <c r="E35" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F35" s="17"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="17"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="17"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17" t="s">
+      <c r="D40" s="16"/>
+      <c r="E40" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="16"/>
     </row>
     <row r="41" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="7"/>
@@ -1219,23 +1219,23 @@
       <c r="B45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17" t="s">
+      <c r="D45" s="16"/>
+      <c r="E45" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="17"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="17"/>
+      <c r="D46" s="16"/>
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
@@ -1245,219 +1245,195 @@
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17" t="s">
+      <c r="D47" s="16"/>
+      <c r="E47" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F47" s="17"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17" t="s">
+      <c r="D48" s="16"/>
+      <c r="E48" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="17"/>
+      <c r="F48" s="16"/>
     </row>
     <row r="49" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17" t="s">
+      <c r="D49" s="16"/>
+      <c r="E49" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F49" s="17"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="17" t="s">
+      <c r="D50" s="17"/>
+      <c r="E50" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F50" s="17"/>
+      <c r="F50" s="16"/>
     </row>
     <row r="51" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F51" s="17"/>
+      <c r="F51" s="16"/>
     </row>
     <row r="52" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17" t="s">
+      <c r="D52" s="16"/>
+      <c r="E52" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="17"/>
+      <c r="F52" s="16"/>
     </row>
     <row r="53" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17" t="s">
+      <c r="D53" s="16"/>
+      <c r="E53" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F53" s="17"/>
+      <c r="F53" s="16"/>
     </row>
     <row r="54" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17" t="s">
+      <c r="D54" s="16"/>
+      <c r="E54" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F54" s="17"/>
+      <c r="F54" s="16"/>
     </row>
     <row r="55" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17" t="s">
+      <c r="D55" s="16"/>
+      <c r="E55" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F55" s="17"/>
+      <c r="F55" s="16"/>
     </row>
     <row r="56" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17" t="s">
+      <c r="D56" s="16"/>
+      <c r="E56" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F56" s="17"/>
+      <c r="F56" s="16"/>
     </row>
     <row r="57" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17" t="s">
+      <c r="D57" s="16"/>
+      <c r="E57" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F57" s="17"/>
+      <c r="F57" s="16"/>
     </row>
     <row r="58" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17" t="s">
+      <c r="D58" s="16"/>
+      <c r="E58" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F58" s="17"/>
+      <c r="F58" s="16"/>
     </row>
     <row r="59" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17" t="s">
+      <c r="D59" s="16"/>
+      <c r="E59" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F59" s="17"/>
+      <c r="F59" s="16"/>
     </row>
     <row r="60" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" s="1" t="s">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="E45:F45"/>
@@ -1474,21 +1450,45 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>